<commit_message>
Refactoring de l'accès aux données. Factorisation. HipBookDataProvider remanié.
</commit_message>
<xml_diff>
--- a/docs/Notes conception. 001.xlsx
+++ b/docs/Notes conception. 001.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="96" windowWidth="12132" windowHeight="5856"/>
+    <workbookView xWindow="672" yWindow="96" windowWidth="12132" windowHeight="5856" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Bibliographic Item" sheetId="1" r:id="rId1"/>
+    <sheet name="Result Set" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Provider" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>title</t>
   </si>
@@ -154,6 +154,94 @@
   </si>
   <si>
     <t>directAccesses</t>
+  </si>
+  <si>
+    <t>currentPage</t>
+  </si>
+  <si>
+    <t>numberOfResults</t>
+  </si>
+  <si>
+    <t>maxResultsPerPage</t>
+  </si>
+  <si>
+    <t>results</t>
+  </si>
+  <si>
+    <t>warningMessage</t>
+  </si>
+  <si>
+    <t>Tableau d'Items</t>
+  </si>
+  <si>
+    <t>Sert à calculer s'il reste des pages de résultats à afficher.</t>
+  </si>
+  <si>
+    <t>Sert à mettre à jour les conteneurs "Stats".</t>
+  </si>
+  <si>
+    <t>Sert à calculer s'il reste des pages de résultats à afficher.
+Sert à calculer s'il s'agit du premier ensemble de résultats pour une nouvelle requête.</t>
+  </si>
+  <si>
+    <t>Sert à indiquer si la source de données demande une requête moins coûteuse.</t>
+  </si>
+  <si>
+    <t>_BASE_URL</t>
+  </si>
+  <si>
+    <t>_MAX_RESULTS_PER_PAGE</t>
+  </si>
+  <si>
+    <t>getSearchResults</t>
+  </si>
+  <si>
+    <t>searchString, pageNumber</t>
+  </si>
+  <si>
+    <t>getDetailedItem</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>_buildRequest</t>
+  </si>
+  <si>
+    <t>_buildResultSet</t>
+  </si>
+  <si>
+    <t>_buildDataItem</t>
+  </si>
+  <si>
+    <t>_buildDetailedDataItem</t>
+  </si>
+  <si>
+    <t>rawXmlData</t>
+  </si>
+  <si>
+    <t>PROPOSITIONS</t>
+  </si>
+  <si>
+    <t>getItemById</t>
+  </si>
+  <si>
+    <t>getNextResults</t>
+  </si>
+  <si>
+    <t>_currentResultPage</t>
+  </si>
+  <si>
+    <t>_currentQuery</t>
+  </si>
+  <si>
+    <t>_currentTotalOfResults</t>
+  </si>
+  <si>
+    <t>Sert à renseigner le maxResultsPerPage des ResultSets.</t>
+  </si>
+  <si>
+    <t>Servait à calculer la catalogUrl des Items.</t>
   </si>
 </sst>
 </file>
@@ -189,8 +277,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -940,24 +1031,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Transfert de responsabilités aux DataProvider (nombre de résultats, existence d'autres résultats), gérant seul l'exploitation des réponses de back-ends. Cela conduit à coupler le code des ResultsArea et des DataProvider.
</commit_message>
<xml_diff>
--- a/docs/Notes conception. 001.xlsx
+++ b/docs/Notes conception. 001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="96" windowWidth="12132" windowHeight="5856" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="672" yWindow="96" windowWidth="12132" windowHeight="5856" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bibliographic Item" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
   <si>
     <t>title</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>buildDetailedDataItem</t>
+  </si>
+  <si>
+    <t>Responsabilité déléguée au DataProvider. Propriété supprimée.</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,31 +1077,40 @@
     <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>49</v>
       </c>
@@ -1106,7 +1118,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>50</v>
       </c>
@@ -1236,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Nombreuses informations supplémentaires récupérées. Nombreuses améliorations graphiques.
</commit_message>
<xml_diff>
--- a/docs/Notes conception. 001.xlsx
+++ b/docs/Notes conception. 001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="96" windowWidth="12132" windowHeight="5856" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="672" yWindow="96" windowWidth="12132" windowHeight="5856"/>
   </bookViews>
   <sheets>
     <sheet name="Bibliographic Item" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>title</t>
   </si>
@@ -94,9 +94,6 @@
     <t>DatabasesSpecificDataSource</t>
   </si>
   <si>
-    <t>directUrl</t>
-  </si>
-  <si>
     <t>holdings</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
   </si>
   <si>
     <t>Prop niv. 2</t>
-  </si>
-  <si>
-    <t>exemplars</t>
   </si>
   <si>
     <t>directAccesses</t>
@@ -276,6 +270,9 @@
   </si>
   <si>
     <t>Responsabilité déléguée au DataProvider. Propriété supprimée.</t>
+  </si>
+  <si>
+    <t>copies</t>
   </si>
 </sst>
 </file>
@@ -639,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,10 +656,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
@@ -686,10 +683,10 @@
         <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -718,7 +715,7 @@
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -738,7 +735,7 @@
         <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -758,7 +755,7 @@
         <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -781,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -789,29 +786,29 @@
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -822,7 +819,7 @@
         <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -839,7 +836,7 @@
         <v>23</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -856,7 +853,7 @@
         <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -864,10 +861,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -922,7 +919,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -934,12 +931,12 @@
         <v>23</v>
       </c>
       <c r="K17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -951,12 +948,12 @@
         <v>23</v>
       </c>
       <c r="K18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -965,12 +962,12 @@
         <v>23</v>
       </c>
       <c r="K19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -979,57 +976,63 @@
         <v>23</v>
       </c>
       <c r="K20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
       </c>
       <c r="K21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>59</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
       </c>
       <c r="G22" t="s">
         <v>23</v>
       </c>
       <c r="K22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G23" t="s">
         <v>23</v>
       </c>
       <c r="K23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
       </c>
       <c r="G24" t="s">
         <v>23</v>
@@ -1038,21 +1041,21 @@
         <v>23</v>
       </c>
       <c r="K24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G25" t="s">
         <v>23</v>
       </c>
       <c r="K25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1067,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1079,51 +1082,51 @@
   <sheetData>
     <row r="2" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
         <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1147,96 +1150,96 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1256,52 +1259,52 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>